<commit_message>
update environmental group descriptions
</commit_message>
<xml_diff>
--- a/documents/Environment_group_table.csv.xlsx
+++ b/documents/Environment_group_table.csv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z3531221_ad_unsw_edu_au/Documents/Antarctica/Antarctica/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2568518F-2229-4D7A-B885-4342C0025FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:40009_{2568518F-2229-4D7A-B885-4342C0025FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C3782A3-692C-4ABC-945E-CCE370578D26}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="240" windowWidth="27750" windowHeight="15225"/>
+    <workbookView xWindow="1050" yWindow="975" windowWidth="27750" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment_group_table" sheetId="1" r:id="rId1"/>
@@ -37,67 +37,67 @@
     <t>Environment 1</t>
   </si>
   <si>
-    <t>Env1</t>
-  </si>
-  <si>
     <t>Environment 2</t>
   </si>
   <si>
-    <t>Env2</t>
-  </si>
-  <si>
     <t>High cliffs, crags, mountainsides, and slopes</t>
   </si>
   <si>
-    <t>High elevation, extremely cold, arid, and rugged ecosystems. Good representation in all mountainous areas, sprinkled among other ecosystems where steep slopes are present. Slopes are too steep to hold snow layer and are typically barren rock with very little biota. Particular subunits cover rugged areas of the peninsula, and all subunits occur in the Transantarctic mountains.</t>
-  </si>
-  <si>
     <t>Environment 3</t>
   </si>
   <si>
-    <t>Env3</t>
-  </si>
-  <si>
-    <t>Warm lowlands</t>
-  </si>
-  <si>
-    <t>Relatively warm, flat/level ecosystems, often coastal but not always. Elevations low and topography is gentle. May be rocky and barren, but often hosts bird colonies and pinnipeds if occurring near the coast.</t>
-  </si>
-  <si>
     <t>Environment 4</t>
   </si>
   <si>
-    <t>Env4</t>
-  </si>
-  <si>
     <t>Environment 5</t>
   </si>
   <si>
-    <t>Env5</t>
-  </si>
-  <si>
     <t>Highland windy plateaus and outcrops</t>
   </si>
   <si>
-    <t xml:space="preserve">Coldest, most arid high-elevation flatlands/plateaus/rounded hills (low ruggedness) with low cloud cover. Characterised especially by high wind. </t>
-  </si>
-  <si>
-    <t>These cold, arid ecosystems occupy a wide range of elevations and terrain types and are characterised by low wind and high levels of solar radiation (typically north-facing)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Occurs on  a broad mid range of elevation and terrain types, usually near or directly on the coast. Characterised by high cloud cover and precipitation, relatively milder climates. Thick snow cover (probably seasonal) remains on the surfaces, which are mostly not steep enough for the snow to slide down. Biota consists mainly of mosses and lichens. Dominates the mountainous areas of the Antarctic peninsula, with representation in the Ellsworth mountains and the westernmost end of the Transantarctic mountains. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mild humid hills and mountains</t>
-  </si>
-  <si>
-    <t>Arid, cold, sunny  hills and mountains</t>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>Midland humid ecosystems</t>
+  </si>
+  <si>
+    <t>Mild lowlands</t>
+  </si>
+  <si>
+    <t>Sunny inclines, mountainsides, nunataks and outcrops</t>
+  </si>
+  <si>
+    <t>Occurs on a broad variety of transitional terrains at low-to-mid elevations, usually near the coast. Characterised by water availability via high cloud cover, snowfall, and melt. Thick snow cover (probably seasonal) remains on the surfaces, which are mostly not steep or windy enough for the snow to slide down. Temperatures are mild and many areas have a substantial growing season. Biota consists mainly of mosses and lichens. Dominates the mountainous areas of the Antarctic peninsula, with representation in the Ellsworth mountains, the Transantarctic mountains, Victoria Land, and Enderby Land.</t>
+  </si>
+  <si>
+    <t>High elevation, extremely cold, arid, and rugged ecosystems receiving low solar radiation (south-facing). Slopes are too steep to hold snow layer and are typically barren rock with very little biota. Occurs sprinkled among other ecosystems where steep slopes are present. Particular subunits cover rugged areas of the peninsula, and all subunits occur in the Transantarctic mountains.</t>
+  </si>
+  <si>
+    <t>Relatively warm ecosystems with gentle relief, often coastal but may extend substantially inland. With especially low elevations, this group contains coastal rocky outcrops, small islands, and beaches as well as flat valley bottoms. May be rocky and barren, but often hosts bird colonies and pinnipeds if occurring near the coast. Occurs all around Antarctica with particular concentrations on the Antarctic Peninsula, in the Transantarctic Mountains, and Victoria Land. Dominates the coastal outcrops around the Eastern margin of the continent.</t>
+  </si>
+  <si>
+    <t>Clear, sunlit (north-facing) rocky slopes with low snow cover. In terms of temperature, water availability, and terrain, E4 is transitional between the milder environments of E1/E3 and the more extreme environments of E2/E5.  Topography and elevation is quite variable. Occurs all over Antarctica with good representation, but particularly dominant in Victoria Land.</t>
+  </si>
+  <si>
+    <t>Very cold and arid high-elevation flatlands/plateaus with low cloud cover. Characterised especially by high winds. Occurs throughout the main continent but is nearly absent from the Antarctic Peninsula.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -575,8 +575,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -633,6 +636,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -931,14 +938,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="95.42578125" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -947,81 +959,81 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D6" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>